<commit_message>
ArrayMap and BinarySearchMap implemented
</commit_message>
<xml_diff>
--- a/BestQuickSorterStatistics.xlsx
+++ b/BestQuickSorterStatistics.xlsx
@@ -2342,6 +2342,20 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:E21" totalsRowShown="0">
+  <autoFilter ref="A1:E21"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="SORTER TYPE"/>
+    <tableColumn id="2" name="LENGTH"/>
+    <tableColumn id="3" name="SWAPS"/>
+    <tableColumn id="4" name="COMPARITIONS"/>
+    <tableColumn id="5" name="NANO TIME"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -2642,10 +2656,15 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -3006,6 +3025,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>